<commit_message>
Table Notes extraceted into other sheet
Co-Authored-By: Sagar Kargathra <9019231+sagarkargathra@users.noreply.github.com>

# Table notes saved as another sheet
</commit_message>
<xml_diff>
--- a/files/1.xlsx
+++ b/files/1.xlsx
@@ -1933,6 +1933,21 @@
           <t>(1994 Onwards)</t>
         </is>
       </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>(1994 Onwards)</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>(1994 Onwards)</t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>(1994 Onwards)</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
@@ -1950,6 +1965,21 @@
           <t>(2012 Onwards)</t>
         </is>
       </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>(2012 Onwards)</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>(2012 Onwards)</t>
+        </is>
+      </c>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>(2012 Onwards)</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
@@ -2031,10 +2061,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="U32:X32"/>
-    <mergeCell ref="U33:X33"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>